<commit_message>
Zaktualizowany wykres Gantta plus zadania
</commit_message>
<xml_diff>
--- a/GANTT.xlsx
+++ b/GANTT.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barte_000\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Zadania</t>
   </si>
@@ -44,32 +39,65 @@
     <t>Zapoznanie się z silnikiem graficznym Unreal Engine</t>
   </si>
   <si>
-    <t>Stworzenie projektu gry</t>
-  </si>
-  <si>
-    <t>Przygotowanie tła gry</t>
-  </si>
-  <si>
-    <t>Ułożenie kilku poziomów gry</t>
-  </si>
-  <si>
-    <t>Wczytanie modeli literek do gry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Odpowiednie oprogramowanie liter </t>
-  </si>
-  <si>
-    <t>Testy</t>
-  </si>
-  <si>
-    <t>Wczytanie pozostałych grafik</t>
+    <t>Napisanie 1 poziomu</t>
+  </si>
+  <si>
+    <t>Napisanie 2 poziomu - to samo co 1 poziom, zmiana prędkości</t>
+  </si>
+  <si>
+    <t>Napisanie 3 poziomu</t>
+  </si>
+  <si>
+    <t>Napisanie 4 poziomu - to samo co 3 poziom, zmiana prędkości</t>
+  </si>
+  <si>
+    <t>Napisanie 6 poziomu - to samo co 5 poziom, zmiana prędkości</t>
+  </si>
+  <si>
+    <t>Wczytanie modeli liter do gry poziom 5 i 6</t>
+  </si>
+  <si>
+    <t>Wczytanie modeli liter do gry poziom 3 i 4</t>
+  </si>
+  <si>
+    <t>Wczytanie modeli liter do gry poziom 1 i 2</t>
+  </si>
+  <si>
+    <t>Testy poziomów</t>
+  </si>
+  <si>
+    <t>Stworzenie GUI</t>
+  </si>
+  <si>
+    <t>Wczytanie pozostałych grafik do gry</t>
+  </si>
+  <si>
+    <t>Testy całości</t>
+  </si>
+  <si>
+    <t>Napisanie dokumentacji</t>
+  </si>
+  <si>
+    <t>Napisanie PostMorten</t>
+  </si>
+  <si>
+    <t>Napisanie 5 poziomu</t>
+  </si>
+  <si>
+    <t>SUMA GODZIN</t>
+  </si>
+  <si>
+    <t>Zrobione</t>
+  </si>
+  <si>
+    <t>þ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +114,12 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -121,6 +155,15 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -188,26 +231,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
@@ -280,9 +303,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$B$3:$B$12</c:f>
+              <c:f>Arkusz1!$B$3:$B$20</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Przygotowanie modelu literek</c:v>
                 </c:pt>
@@ -293,35 +316,59 @@
                   <c:v>Zapoznanie się z silnikiem graficznym Unreal Engine</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Stworzenie projektu gry</c:v>
+                  <c:v>Wczytanie modeli liter do gry poziom 1 i 2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Przygotowanie tła gry</c:v>
+                  <c:v>Napisanie 1 poziomu</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Ułożenie kilku poziomów gry</c:v>
+                  <c:v>Napisanie 2 poziomu - to samo co 1 poziom, zmiana prędkości</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Wczytanie modeli literek do gry</c:v>
+                  <c:v>Wczytanie modeli liter do gry poziom 3 i 4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Odpowiednie oprogramowanie liter </c:v>
+                  <c:v>Napisanie 3 poziomu</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Testy</c:v>
+                  <c:v>Napisanie 4 poziomu - to samo co 3 poziom, zmiana prędkości</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Wczytanie pozostałych grafik</c:v>
+                  <c:v>Wczytanie modeli liter do gry poziom 5 i 6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Napisanie 5 poziomu</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Napisanie 6 poziomu - to samo co 5 poziom, zmiana prędkości</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Testy poziomów</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Stworzenie GUI</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Wczytanie pozostałych grafik do gry</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Testy całości</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Napisanie dokumentacji</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Napisanie PostMorten</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$3:$C$12</c:f>
+              <c:f>Arkusz1!$C$3:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42819</c:v>
                 </c:pt>
@@ -329,13 +376,13 @@
                   <c:v>42823</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42826</c:v>
+                  <c:v>42828</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42827</c:v>
+                  <c:v>42832</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42830</c:v>
+                  <c:v>42832</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>42833</c:v>
@@ -344,13 +391,37 @@
                   <c:v>42833</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>42833</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42833</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42833</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42833</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42833</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42833</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42833</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>42834</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>42837</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>42837</c:v>
+                <c:pt idx="15">
+                  <c:v>42834</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42835</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -383,9 +454,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$B$3:$B$12</c:f>
+              <c:f>Arkusz1!$B$3:$B$20</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Przygotowanie modelu literek</c:v>
                 </c:pt>
@@ -396,35 +467,59 @@
                   <c:v>Zapoznanie się z silnikiem graficznym Unreal Engine</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Stworzenie projektu gry</c:v>
+                  <c:v>Wczytanie modeli liter do gry poziom 1 i 2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Przygotowanie tła gry</c:v>
+                  <c:v>Napisanie 1 poziomu</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Ułożenie kilku poziomów gry</c:v>
+                  <c:v>Napisanie 2 poziomu - to samo co 1 poziom, zmiana prędkości</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Wczytanie modeli literek do gry</c:v>
+                  <c:v>Wczytanie modeli liter do gry poziom 3 i 4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Odpowiednie oprogramowanie liter </c:v>
+                  <c:v>Napisanie 3 poziomu</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Testy</c:v>
+                  <c:v>Napisanie 4 poziomu - to samo co 3 poziom, zmiana prędkości</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Wczytanie pozostałych grafik</c:v>
+                  <c:v>Wczytanie modeli liter do gry poziom 5 i 6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Napisanie 5 poziomu</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Napisanie 6 poziomu - to samo co 5 poziom, zmiana prędkości</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Testy poziomów</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Stworzenie GUI</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Wczytanie pozostałych grafik do gry</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Testy całości</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Napisanie dokumentacji</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Napisanie PostMorten</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$D$3:$D$12</c:f>
+              <c:f>Arkusz1!$D$3:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -435,25 +530,49 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.5</c:v>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -470,12 +589,12 @@
         <c:gapWidth val="95"/>
         <c:gapDepth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="84492840"/>
-        <c:axId val="84494016"/>
+        <c:axId val="144363520"/>
+        <c:axId val="144365056"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="84492840"/>
+        <c:axId val="144363520"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -512,7 +631,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84494016"/>
+        <c:crossAx val="144365056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -520,10 +639,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84494016"/>
+        <c:axId val="144365056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="42820"/>
+          <c:max val="42843"/>
+          <c:min val="42818"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -572,7 +692,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84492840"/>
+        <c:crossAx val="144363520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1198,16 +1318,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2228849</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228598</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1484,7 +1604,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1492,19 +1612,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I13"/>
+  <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="53" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1518,6 +1639,9 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1529,8 +1653,11 @@
       <c r="D3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1539,6 +1666,9 @@
       </c>
       <c r="D4" s="1">
         <v>3</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -1546,100 +1676,232 @@
         <v>5</v>
       </c>
       <c r="C5" s="3">
-        <v>42826</v>
+        <v>42828</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="I5" s="4">
-        <v>42823</v>
-      </c>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3">
-        <v>42827</v>
+        <v>42832</v>
       </c>
       <c r="D6" s="1">
-        <v>8</v>
-      </c>
-      <c r="I6" s="4">
-        <v>42820</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>42832</v>
+      </c>
+      <c r="D7" s="1">
         <v>7</v>
       </c>
-      <c r="C7" s="3">
-        <v>42830</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.5</v>
+      <c r="E7" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3">
         <v>42833</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3">
         <v>42833</v>
       </c>
       <c r="D9" s="1">
-        <v>0.5</v>
+        <v>2</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
-        <v>42834</v>
+        <v>42833</v>
       </c>
       <c r="D10" s="1">
-        <v>2.5</v>
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3">
-        <v>42837</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2</v>
+        <v>42833</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3">
-        <v>42837</v>
+        <v>42833</v>
       </c>
       <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3">
+        <v>42833</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3">
+        <v>42833</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3">
+        <v>42833</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>42833</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3">
+        <v>42834</v>
+      </c>
+      <c r="D17" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="1">
-        <f>SUM(D4,D5,D6,D7,D8,D9,D10,D11,D12)</f>
-        <v>20.5</v>
-      </c>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3">
+        <v>42834</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3">
+        <v>42835</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3">
+        <v>42835</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="5">
+        <f>SUM(D3:D20)</f>
+        <v>39.503333333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Działająca gra bez wczytanych grafik układu palców na klawiaturze.
</commit_message>
<xml_diff>
--- a/GANTT.xlsx
+++ b/GANTT.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barte_000\Documents\Unreal Projects\Nowy folder\Klawiaturka\klawiatura\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Zadania</t>
   </si>
@@ -78,9 +83,6 @@
     <t>Napisanie dokumentacji</t>
   </si>
   <si>
-    <t>Napisanie PostMorten</t>
-  </si>
-  <si>
     <t>Napisanie 5 poziomu</t>
   </si>
   <si>
@@ -91,6 +93,9 @@
   </si>
   <si>
     <t>þ</t>
+  </si>
+  <si>
+    <t>Napisanie Post Mortem</t>
   </si>
 </sst>
 </file>
@@ -231,6 +236,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
@@ -358,7 +383,7 @@
                   <c:v>Napisanie dokumentacji</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Napisanie PostMorten</c:v>
+                  <c:v>Napisanie Post Mortem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -509,7 +534,7 @@
                   <c:v>Napisanie dokumentacji</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Napisanie PostMorten</c:v>
+                  <c:v>Napisanie Post Mortem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -589,12 +614,12 @@
         <c:gapWidth val="95"/>
         <c:gapDepth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="144363520"/>
-        <c:axId val="144365056"/>
+        <c:axId val="155166920"/>
+        <c:axId val="155169664"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="144363520"/>
+        <c:axId val="155166920"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -631,7 +656,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144365056"/>
+        <c:crossAx val="155169664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -639,7 +664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144365056"/>
+        <c:axId val="155169664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42843"/>
@@ -692,7 +717,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144363520"/>
+        <c:crossAx val="155166920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1604,7 +1629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1615,7 +1640,7 @@
   <dimension ref="B1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,7 +1665,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -1654,7 +1679,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -1668,7 +1693,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -1682,7 +1707,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="4"/>
     </row>
@@ -1697,7 +1722,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -1712,7 +1737,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -1726,7 +1751,7 @@
         <v>0.17</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1740,7 +1765,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -1754,7 +1779,7 @@
         <v>1.5</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -1768,7 +1793,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -1782,12 +1807,12 @@
         <v>2</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3">
         <v>42833</v>
@@ -1796,7 +1821,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -1810,7 +1835,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -1824,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -1837,7 +1862,9 @@
       <c r="D16" s="1">
         <v>3</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -1877,7 +1904,7 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C20" s="3">
         <v>42835</v>
@@ -1889,7 +1916,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="5">

</xml_diff>

<commit_message>
Zaktualizowany plik excel - zadania i wykres Gantta
</commit_message>
<xml_diff>
--- a/GANTT.xlsx
+++ b/GANTT.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barte_000\Documents\Unreal Projects\Nowy folder\Klawiaturka\klawiatura\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Zadania</t>
   </si>
@@ -236,26 +231,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
@@ -434,19 +409,19 @@
                   <c:v>42833</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42833</c:v>
+                  <c:v>42834</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>42834</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42834</c:v>
+                  <c:v>42835</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42835</c:v>
+                  <c:v>42836</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42835</c:v>
+                  <c:v>42836</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -614,12 +589,12 @@
         <c:gapWidth val="95"/>
         <c:gapDepth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="155166920"/>
-        <c:axId val="155169664"/>
+        <c:axId val="186896384"/>
+        <c:axId val="186897920"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="155166920"/>
+        <c:axId val="186896384"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -656,7 +631,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="155169664"/>
+        <c:crossAx val="186897920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -664,7 +639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155169664"/>
+        <c:axId val="186897920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42843"/>
@@ -717,7 +692,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="155166920"/>
+        <c:crossAx val="186896384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1629,7 +1604,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1639,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,7 +1832,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="3">
-        <v>42833</v>
+        <v>42834</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>
@@ -1876,26 +1851,30 @@
       <c r="D17" s="1">
         <v>0.5</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="3">
-        <v>42834</v>
+        <v>42835</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="3">
-        <v>42835</v>
+        <v>42836</v>
       </c>
       <c r="D19" s="1">
         <v>5</v>
@@ -1907,7 +1886,7 @@
         <v>23</v>
       </c>
       <c r="C20" s="3">
-        <v>42835</v>
+        <v>42836</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>

</xml_diff>